<commit_message>
Profils OncoFAIRPatient et OncoFAIREncounter e218ae366944634f18ff4e9ed414eda764f7f6e6
</commit_message>
<xml_diff>
--- a/mapping-pn13/ig/StructureDefinition-oncofair-patient.xlsx
+++ b/mapping-pn13/ig/StructureDefinition-oncofair-patient.xlsx
@@ -9,6 +9,9 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$46</definedName>
+  </definedNames>
 </workbook>
 </file>
 
@@ -57,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-19T08:32:40+00:00</t>
+    <t>2024-04-22T07:26:57+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -487,7 +490,7 @@
 </t>
   </si>
   <si>
-    <t>An identifier for this patient</t>
+    <t>The patient's identifier</t>
   </si>
   <si>
     <t>An identifier for this patient.</t>
@@ -1334,6 +1337,21 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="22"/>
+        <i val="true"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -1682,7 +1700,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
         <v>28</v>
       </c>
@@ -1800,7 +1818,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
         <v>89</v>
       </c>
@@ -1920,7 +1938,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
         <v>97</v>
       </c>
@@ -2038,7 +2056,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
         <v>103</v>
       </c>
@@ -2158,7 +2176,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
         <v>109</v>
       </c>
@@ -2278,7 +2296,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
         <v>118</v>
       </c>
@@ -2398,7 +2416,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
         <v>127</v>
       </c>
@@ -2518,7 +2536,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
         <v>136</v>
       </c>
@@ -2638,7 +2656,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
         <v>144</v>
       </c>
@@ -2760,7 +2778,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
         <v>149</v>
       </c>
@@ -2773,13 +2791,13 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s" s="2">
         <v>79</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>80</v>
@@ -2880,7 +2898,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
         <v>159</v>
       </c>
@@ -3004,7 +3022,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
         <v>170</v>
       </c>
@@ -3126,7 +3144,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
         <v>180</v>
       </c>
@@ -3248,7 +3266,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
         <v>190</v>
       </c>
@@ -3370,7 +3388,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
         <v>201</v>
       </c>
@@ -3492,7 +3510,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
         <v>212</v>
       </c>
@@ -3614,7 +3632,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
         <v>220</v>
       </c>
@@ -3736,7 +3754,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
         <v>230</v>
       </c>
@@ -3856,7 +3874,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
         <v>241</v>
       </c>
@@ -3978,7 +3996,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
         <v>249</v>
       </c>
@@ -4100,7 +4118,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
         <v>258</v>
       </c>
@@ -4222,7 +4240,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
         <v>266</v>
       </c>
@@ -4340,7 +4358,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
         <v>272</v>
       </c>
@@ -4460,7 +4478,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
         <v>275</v>
       </c>
@@ -4582,7 +4600,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
         <v>280</v>
       </c>
@@ -4702,7 +4720,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
         <v>288</v>
       </c>
@@ -4822,7 +4840,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
         <v>294</v>
       </c>
@@ -4944,7 +4962,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
         <v>299</v>
       </c>
@@ -5064,7 +5082,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
         <v>304</v>
       </c>
@@ -5184,7 +5202,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
         <v>308</v>
       </c>
@@ -5304,7 +5322,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
         <v>315</v>
       </c>
@@ -5422,7 +5440,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
         <v>320</v>
       </c>
@@ -5544,7 +5562,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
         <v>328</v>
       </c>
@@ -5662,7 +5680,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
         <v>329</v>
       </c>
@@ -5782,7 +5800,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
         <v>330</v>
       </c>
@@ -5904,7 +5922,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
         <v>331</v>
       </c>
@@ -6026,7 +6044,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
         <v>339</v>
       </c>
@@ -6148,7 +6166,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
         <v>347</v>
       </c>
@@ -6268,7 +6286,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
         <v>355</v>
       </c>
@@ -6390,7 +6408,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
         <v>361</v>
       </c>
@@ -6512,7 +6530,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
         <v>367</v>
       </c>
@@ -6630,7 +6648,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
         <v>368</v>
       </c>
@@ -6750,7 +6768,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
         <v>369</v>
       </c>
@@ -6872,7 +6890,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
         <v>370</v>
       </c>
@@ -6992,7 +7010,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
         <v>375</v>
       </c>
@@ -7111,6 +7129,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AP46">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="26">
+      <filters blank="true"/>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="A2:AI45">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G2&lt;&gt;"Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$Q2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>